<commit_message>
Added logic to write result to excel file
</commit_message>
<xml_diff>
--- a/person_generator.xlsx
+++ b/person_generator.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tanikawa\workspace\person-generator\person-generator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02DAA5F1-2B1D-440A-9497-4782331ACA8F}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF9CCC06-AA99-43D6-B693-B1A0C594AF25}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="9990" xr2:uid="{0532160E-D53B-456B-9F30-3F35FB680C00}"/>
   </bookViews>
@@ -7049,7 +7049,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B13" sqref="B13"/>
+      <selection pane="bottomRight" activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
@@ -7078,11 +7078,12 @@
         <v>1994</v>
       </c>
     </row>
+    <row r="2" spans="1:5" ht="18.5" thickBot="1" x14ac:dyDescent="0.6"/>
     <row r="3" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>2017</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="15" t="s">
         <v>2016</v>
       </c>
       <c r="C3">

</xml_diff>